<commit_message>
upload sql_scr2 and sql regulation excel
</commit_message>
<xml_diff>
--- a/SQL/SQL評量_正規化題目.xlsx
+++ b/SQL/SQL評量_正規化題目.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Java班\git_upload\SQL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EBCB54D8-0E11-4A2D-8DE9-B2B8E3CA9CD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BE6B77A-0810-40FF-B125-B03EB4CD5B98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{36CE15E8-7DE5-4D3C-B6E0-1B1AB355C8A4}"/>
   </bookViews>
@@ -20,12 +20,21 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="149">
   <si>
     <r>
       <rPr>
@@ -1465,96 +1474,415 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>類別</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>村里ID</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>村里辦公室地址</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>村里辦公室電話</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>設施ID</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>P01</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>P02</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>P03</t>
-  </si>
-  <si>
-    <t>P04</t>
-  </si>
-  <si>
-    <t>P05</t>
-  </si>
-  <si>
-    <t>P06</t>
-  </si>
-  <si>
-    <t>P07</t>
-  </si>
-  <si>
-    <t>P08</t>
-  </si>
-  <si>
-    <t>P09</t>
-  </si>
-  <si>
-    <t>P10</t>
-  </si>
-  <si>
-    <t>A001</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>A002</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>A003</t>
-  </si>
-  <si>
-    <t>A004</t>
-  </si>
-  <si>
-    <t>A005</t>
-  </si>
-  <si>
     <t>FK</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>村里別</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>類別ID</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>苗栗縣竹南鎮中埔街</t>
+    <t>警察轄區表(POLICE)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>村里表(VILLAGE)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>苗栗縣警察局防空疏散避難設施表(MIAOLI_EVACUATION_FACILITY)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>竹南鎮民族街</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>72</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>號</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>苗栗市金鳳街</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>109</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>號</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>頭份市中興路</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>503</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>號</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>竹南鎮</t>
+  </si>
+  <si>
+    <t>後龍鎮</t>
+  </si>
+  <si>
+    <t>苗栗市</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>公義路</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>1035</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>號</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>頭份市</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>中山路</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 103 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>號</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>國光街</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 14 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>號</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>中興路</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>136-1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>號</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>中正路</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 766 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>號</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>民族路</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>96</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>號</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>光大街</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>82</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>號</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>信義路</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>53</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>巷</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>號</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>中埔街</t>
     </r>
     <r>
       <rPr>
@@ -1586,7 +1914,7 @@
         <family val="2"/>
         <charset val="136"/>
       </rPr>
-      <t>苗栗縣竹南鎮和平街</t>
+      <t>和平街</t>
     </r>
     <r>
       <rPr>
@@ -1618,7 +1946,7 @@
         <family val="2"/>
         <charset val="136"/>
       </rPr>
-      <t>苗栗縣竹南鎮龍山路三段</t>
+      <t>龍山路三段</t>
     </r>
     <r>
       <rPr>
@@ -1650,7 +1978,7 @@
         <family val="2"/>
         <charset val="136"/>
       </rPr>
-      <t>苗栗縣後龍鎮中華路</t>
+      <t>中華路</t>
     </r>
     <r>
       <rPr>
@@ -1675,7 +2003,7 @@
   </si>
   <si>
     <r>
-      <t>苗栗縣苗栗市米市街</t>
+      <t>米市街</t>
     </r>
     <r>
       <rPr>
@@ -1707,7 +2035,7 @@
         <family val="2"/>
         <charset val="136"/>
       </rPr>
-      <t>苗栗縣苗栗市光復路</t>
+      <t>光復路</t>
     </r>
     <r>
       <rPr>
@@ -1732,7 +2060,7 @@
   </si>
   <si>
     <r>
-      <t>苗栗縣苗栗市博愛街</t>
+      <t>博愛街</t>
     </r>
     <r>
       <rPr>
@@ -1765,7 +2093,7 @@
         <family val="2"/>
         <charset val="136"/>
       </rPr>
-      <t>苗栗縣苗栗市大同路</t>
+      <t>大同路</t>
     </r>
     <r>
       <rPr>
@@ -1797,7 +2125,71 @@
         <family val="2"/>
         <charset val="136"/>
       </rPr>
-      <t>苗栗縣頭份市民族里和平路</t>
+      <t>中正路</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>116</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>號</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>中正路</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>65</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>號</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>和平路</t>
     </r>
     <r>
       <rPr>
@@ -1829,7 +2221,7 @@
         <family val="2"/>
         <charset val="136"/>
       </rPr>
-      <t>苗栗縣頭份市忠孝忠孝一路</t>
+      <t>忠孝一路</t>
     </r>
     <r>
       <rPr>
@@ -1853,91 +2245,185 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>苗栗縣頭份市信義里中正路</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>65</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>號</t>
-    </r>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>苗栗縣頭份市信義里中正路</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>116</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="微軟正黑體"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t>號</t>
-    </r>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>警察轄區表(POLICE)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>村里表(VILLAGE)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>設施類別表(FACILITY)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>苗栗縣警察局防空疏散避難設施表(MIAOLI_EVACUATION_FACILITY)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>容人數量</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>設施地址</t>
+    <t>P001</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>P002</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>P003</t>
+  </si>
+  <si>
+    <t>P004</t>
+  </si>
+  <si>
+    <t>P005</t>
+  </si>
+  <si>
+    <t>P006</t>
+  </si>
+  <si>
+    <t>P007</t>
+  </si>
+  <si>
+    <t>P008</t>
+  </si>
+  <si>
+    <t>P009</t>
+  </si>
+  <si>
+    <t>P010</t>
+  </si>
+  <si>
+    <t>P011</t>
+  </si>
+  <si>
+    <t>P012</t>
+  </si>
+  <si>
+    <t>C001</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>037-581072</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>竹南分局</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>M001</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>苗栗分局</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>頭份分局</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>03 747 4796</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>03 732 0059</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>03 766 3004</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>FK</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>CHAR(4 BYTE)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ID</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>NVARCHAR2(10)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>NVARCHAR2(5)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>NVARCHAR2(50)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>VARCHAR2(20)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>char(4 BYTE)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>NAME</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>TOWN</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADDRESS</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>TEL</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ID</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>NAME</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADDRESS</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">CATEGORY </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">VIL_ID </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">TOWN </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">ADDRESS </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">FLOOR_NUM </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">PS_ID </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">CAPACITY </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">CHAR(4 BYTE) </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>NVARCHAR2(8)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>大樓</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">CHAR(4 Byte) </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1984,19 +2470,20 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="新細明體"/>
-      <family val="2"/>
+      <name val="細明體"/>
+      <family val="3"/>
       <charset val="136"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="細明體"/>
-      <family val="3"/>
+      <name val="新細明體"/>
+      <family val="1"/>
       <charset val="136"/>
+      <scheme val="major"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2015,8 +2502,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -2039,50 +2550,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2095,50 +2569,62 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2454,10 +2940,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF1A47CA-532C-4318-8D23-1C0A59A513C2}">
-  <dimension ref="A1:L43"/>
+  <dimension ref="A1:M45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17:L17"/>
+    <sheetView tabSelected="1" topLeftCell="C16" workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -2466,14 +2952,15 @@
     <col min="2" max="2" width="11.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.625" customWidth="1"/>
     <col min="4" max="4" width="37.375" customWidth="1"/>
-    <col min="5" max="5" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.125" customWidth="1"/>
     <col min="6" max="6" width="39.625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.375" customWidth="1"/>
     <col min="8" max="8" width="21.75" customWidth="1"/>
     <col min="9" max="9" width="14.875" customWidth="1"/>
     <col min="10" max="10" width="26.125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27.5" customWidth="1"/>
-    <col min="12" max="12" width="14" customWidth="1"/>
+    <col min="11" max="11" width="15.25" customWidth="1"/>
+    <col min="12" max="12" width="20.875" customWidth="1"/>
+    <col min="13" max="13" width="13.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -2861,626 +3348,718 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="B17" s="4"/>
-      <c r="D17" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="10"/>
-      <c r="I17" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="13"/>
+      <c r="B17" s="13"/>
+      <c r="D17" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="J17" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="K17" s="18"/>
+      <c r="L17" s="18"/>
+      <c r="M17" s="18"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="12"/>
+      <c r="B18" s="12"/>
+      <c r="D18" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="B18" s="5"/>
-      <c r="D18" s="5" t="s">
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
+      <c r="J18" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="I18" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="I19" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="J19" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="K19" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="L19" s="11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+      <c r="K18" s="22"/>
+      <c r="L18" s="22"/>
+      <c r="M18" s="22"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="12"/>
+      <c r="B19" s="12"/>
+      <c r="D19" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="F19" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="G19" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="H19" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="J19" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="K19" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="L19" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="M19" s="19" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="12"/>
+      <c r="B20" s="12"/>
+      <c r="D20" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="E20" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="F20" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="G20" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="H20" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="J20" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="K20" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="L20" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="M20" s="20" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="10"/>
+      <c r="B21" s="11"/>
+      <c r="D21" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="J21" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="K21" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="L21" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="M21" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="10"/>
+      <c r="B22" s="11"/>
+      <c r="D22" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="J22" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="K22" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="L22" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="M22" s="5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="10"/>
+      <c r="B23" s="11"/>
+      <c r="D23" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J23" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="K23" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="L23" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="M23" s="5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="10"/>
+      <c r="B24" s="11"/>
+      <c r="D24" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="10"/>
+      <c r="B25" s="11"/>
+      <c r="D25" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G25" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="B20" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G20" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="I20" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J20" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="K20" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="L20" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
+      <c r="H25" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D26" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="G26" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="B21" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I21" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="J21" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="K21" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="L21" s="7" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+      <c r="H26" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D27" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="G27" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="B22" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="F22" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="G22" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="I22" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="J22" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="K22" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="L22" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
+      <c r="H27" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D28" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="G28" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="B23" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="G23" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="F24" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="G24" s="7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D25" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="G25" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
-      <c r="L25" s="2"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D26" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="F26" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="G26" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D27" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="E27" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="G27" s="7" t="s">
+      <c r="H28" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
-      <c r="L27" s="2"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="8" t="s">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="B30" s="18"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
+      <c r="H30" s="18"/>
+      <c r="L30" s="2"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="B31" s="19"/>
+      <c r="C31" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="D31" s="19"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="H31" s="19"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="B32" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="C32" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="D32" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="E32" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="F32" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="G32" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="H32" s="19" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="B33" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="C33" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="D33" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="E33" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="F33" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="G33" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="H33" s="20" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="F34" s="5">
+        <v>1</v>
+      </c>
+      <c r="G34" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="H34" s="5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="C35" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="F35" s="5">
+        <v>1</v>
+      </c>
+      <c r="G35" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="H35" s="5">
+        <v>3142</v>
+      </c>
+      <c r="I35" s="2"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C36" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="F36" s="5">
+        <v>1</v>
+      </c>
+      <c r="G36" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="H36" s="5">
+        <v>1072</v>
+      </c>
+      <c r="I36" s="2"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C37" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F37" s="5">
+        <v>1</v>
+      </c>
+      <c r="G37" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="H37" s="5">
+        <v>32</v>
+      </c>
+      <c r="I37" s="2"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="F38" s="5">
+        <v>1</v>
+      </c>
+      <c r="G38" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="H38" s="5">
+        <v>106</v>
+      </c>
+      <c r="I38" s="2"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C39" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="F39" s="5">
+        <v>1</v>
+      </c>
+      <c r="G39" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="H39" s="5">
+        <v>26</v>
+      </c>
+      <c r="I39" s="2"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C40" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="F40" s="5">
+        <v>2</v>
+      </c>
+      <c r="G40" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="H40" s="5">
+        <v>2038</v>
+      </c>
+      <c r="I40" s="2"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="B29" s="9"/>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="12"/>
-      <c r="I29" s="12"/>
-      <c r="J29" s="12"/>
-      <c r="K29" s="12"/>
-      <c r="L29" s="2"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="G30" s="5"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="B31" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C31" s="11" t="s">
+      <c r="B41" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C41" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="F41" s="5">
+        <v>2</v>
+      </c>
+      <c r="G41" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="H41" s="5">
+        <v>128</v>
+      </c>
+      <c r="I41" s="2"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C42" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="F42" s="5">
         <v>1</v>
       </c>
-      <c r="D31" s="18" t="s">
+      <c r="G42" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="H42" s="5">
+        <v>353</v>
+      </c>
+      <c r="I42" s="2"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="E31" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="F31" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="G31" s="17" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D32" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="E32" s="7">
+      <c r="B43" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C43" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="F43" s="5">
         <v>1</v>
       </c>
-      <c r="F32" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G32" s="7">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D33" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="E33" s="7">
+      <c r="G43" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="H43" s="5">
+        <v>501</v>
+      </c>
+      <c r="I43" s="2"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C44" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="F44" s="5">
         <v>1</v>
       </c>
-      <c r="F33" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G33" s="7">
-        <v>3142</v>
-      </c>
-      <c r="I33" s="2"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D34" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="E34" s="7">
+      <c r="G44" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="H44" s="5">
+        <v>194</v>
+      </c>
+      <c r="I44" s="2"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C45" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="F45" s="5">
         <v>1</v>
       </c>
-      <c r="F34" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G34" s="7">
-        <v>1072</v>
-      </c>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="6" t="s">
+      <c r="G45" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="H45" s="5">
         <v>78</v>
       </c>
-      <c r="B35" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D35" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="E35" s="7">
-        <v>1</v>
-      </c>
-      <c r="F35" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G35" s="7">
-        <v>32</v>
-      </c>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="C36" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D36" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="E36" s="7">
-        <v>1</v>
-      </c>
-      <c r="F36" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="G36" s="7">
-        <v>106</v>
-      </c>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D37" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="E37" s="7">
-        <v>1</v>
-      </c>
-      <c r="F37" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="G37" s="7">
-        <v>26</v>
-      </c>
-      <c r="H37" s="2"/>
-      <c r="I37" s="2"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="B38" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="C38" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D38" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="E38" s="7">
-        <v>2</v>
-      </c>
-      <c r="F38" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="G38" s="7">
-        <v>2038</v>
-      </c>
-      <c r="I38" s="2"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D39" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="E39" s="7">
-        <v>2</v>
-      </c>
-      <c r="F39" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="G39" s="7">
-        <v>128</v>
-      </c>
-      <c r="H39" s="2"/>
-      <c r="I39" s="2"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="B40" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="C40" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D40" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="E40" s="7">
-        <v>1</v>
-      </c>
-      <c r="F40" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="G40" s="7">
-        <v>353</v>
-      </c>
-      <c r="H40" s="2"/>
-      <c r="I40" s="2"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="B41" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="D41" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="E41" s="7">
-        <v>1</v>
-      </c>
-      <c r="F41" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="G41" s="7">
-        <v>501</v>
-      </c>
-      <c r="H41" s="2"/>
-      <c r="I41" s="2"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="B42" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="C42" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D42" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="E42" s="7">
-        <v>1</v>
-      </c>
-      <c r="F42" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="G42" s="7">
-        <v>194</v>
-      </c>
-      <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="B43" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="C43" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D43" s="13" t="s">
-        <v>104</v>
-      </c>
-      <c r="E43" s="7">
-        <v>1</v>
-      </c>
-      <c r="F43" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="G43" s="7">
-        <v>78</v>
-      </c>
-      <c r="H43" s="2"/>
-      <c r="I43" s="2"/>
+      <c r="I45" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="D17:G17"/>
-    <mergeCell ref="I17:L17"/>
-    <mergeCell ref="A29:G29"/>
+  <mergeCells count="3">
+    <mergeCell ref="J17:M17"/>
+    <mergeCell ref="A30:H30"/>
+    <mergeCell ref="D17:H17"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>